<commit_message>
feature/visit-group: add characteristic the group visit
</commit_message>
<xml_diff>
--- a/assets/template/visit.xlsx
+++ b/assets/template/visit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\fablab-system\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBF38CB-FFFB-48A4-9B85-A0BA7D19E37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEF84EF-E9F6-4761-BDE2-1A87800499F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="1224" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t>tipo_documento</t>
   </si>
@@ -55,13 +55,46 @@
   </si>
   <si>
     <t>corregimiento</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>jesus agudo</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>jagudo2514@mgil.aocm</t>
+  </si>
+  <si>
+    <t>jagudo25@asja.com</t>
+  </si>
+  <si>
+    <t>sdsdsd@afjjsd.com</t>
+  </si>
+  <si>
+    <t>samdkasjd@gjjs.com</t>
+  </si>
+  <si>
+    <t>asmdjasjd@ksdk.com</t>
+  </si>
+  <si>
+    <t>Veraguas</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>9-755-1542</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,16 +102,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -86,15 +139,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Notas" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -372,18 +446,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
     <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" customWidth="1"/>
+    <col min="7" max="7" width="33.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -397,16 +477,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -418,7 +498,174 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>232323</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>2326</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>19</v>
+      </c>
+      <c r="F3">
+        <v>43434</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2327</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>34345</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>2358</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>343443</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>2323</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>4343432</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{E90CF8D3-52AF-4133-A213-9D250BE2DEAE}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{B952A0C0-436D-4F4F-B403-89627FB1B054}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{6536CAE0-A6C7-4A67-915C-FEE2228D316D}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{FC0CFAA7-DC1F-4CFF-85EE-D807D65EF8FC}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{4818DB2D-8A43-42F2-9EF4-C84C32C7D476}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>